<commit_message>
Metodos de eliminar ventas en base de datos y remover bloques en la vista
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
   <si>
     <t>Guia</t>
   </si>
@@ -351,15 +351,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -392,16 +432,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -417,16 +447,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -730,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +810,7 @@
         <v>29</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H55" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="H2:H62" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -1387,10 +1407,10 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>2005325438</v>
+        <v>2005325437</v>
       </c>
       <c r="B30" s="5">
-        <v>302158993</v>
+        <v>302158992</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>37</v>
@@ -1414,10 +1434,10 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>2005325439</v>
+        <v>2005325437</v>
       </c>
       <c r="B31" s="5">
-        <v>302158994</v>
+        <v>302158992</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>38</v>
@@ -1441,10 +1461,10 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
-        <v>2005325440</v>
+        <v>2005325437</v>
       </c>
       <c r="B32" s="5">
-        <v>302158995</v>
+        <v>302158992</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>39</v>
@@ -1644,7 +1664,7 @@
       <c r="E39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="8"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
@@ -1667,7 +1687,7 @@
       <c r="E40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="8"/>
+      <c r="F40" s="7"/>
       <c r="H40" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1689,7 +1709,7 @@
       <c r="E41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="8"/>
+      <c r="F41" s="7"/>
       <c r="H41" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1711,7 +1731,7 @@
       <c r="E42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="8"/>
+      <c r="F42" s="7"/>
       <c r="H42" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1990,26 +2010,179 @@
         <v>1</v>
       </c>
     </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <v>2005325464</v>
+      </c>
+      <c r="B56" s="5">
+        <v>302159019</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>2005325465</v>
+      </c>
+      <c r="B57" s="5">
+        <v>302159020</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+      <c r="H57" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="5">
+        <v>2005325466</v>
+      </c>
+      <c r="B58" s="5">
+        <v>302159021</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <v>2005325467</v>
+      </c>
+      <c r="B59" s="5">
+        <v>302159022</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>29</v>
+      </c>
+      <c r="H59" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>2005325468</v>
+      </c>
+      <c r="B60" s="5">
+        <v>302159023</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>29</v>
+      </c>
+      <c r="H60" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="5">
+        <v>2005325469</v>
+      </c>
+      <c r="B61" s="5">
+        <v>302159024</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H61" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
+        <v>2005325470</v>
+      </c>
+      <c r="B62" s="5">
+        <v>302159025</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B55">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="B2:B62">
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:C53">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C61">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C62">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2031,10 +2204,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
insertar estado de aenvio al no procesar una venta
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
   <si>
     <t>Guia</t>
   </si>
@@ -351,15 +351,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -392,16 +402,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -422,31 +422,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -750,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +790,7 @@
         <v>29</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H62" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="H2:H55" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -1407,10 +1387,10 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>2005325437</v>
+        <v>2005325438</v>
       </c>
       <c r="B30" s="5">
-        <v>302158992</v>
+        <v>302158993</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>37</v>
@@ -1434,10 +1414,10 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>2005325437</v>
+        <v>2005325439</v>
       </c>
       <c r="B31" s="5">
-        <v>302158992</v>
+        <v>302158994</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>38</v>
@@ -1461,10 +1441,10 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
-        <v>2005325437</v>
+        <v>2005325440</v>
       </c>
       <c r="B32" s="5">
-        <v>302158992</v>
+        <v>302158995</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>39</v>
@@ -1664,7 +1644,7 @@
       <c r="E39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="7"/>
+      <c r="F39" s="8"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
@@ -1687,7 +1667,7 @@
       <c r="E40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="8"/>
       <c r="H40" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1709,7 +1689,7 @@
       <c r="E41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="8"/>
       <c r="H41" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1731,7 +1711,7 @@
       <c r="E42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="8"/>
       <c r="H42" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2010,179 +1990,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5">
-        <v>2005325464</v>
-      </c>
-      <c r="B56" s="5">
-        <v>302159019</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>31</v>
-      </c>
-      <c r="H56" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5">
-        <v>2005325465</v>
-      </c>
-      <c r="B57" s="5">
-        <v>302159020</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57">
-        <v>3</v>
-      </c>
-      <c r="E57" t="s">
-        <v>31</v>
-      </c>
-      <c r="H57" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5">
-        <v>2005325466</v>
-      </c>
-      <c r="B58" s="5">
-        <v>302159021</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58">
-        <v>4</v>
-      </c>
-      <c r="E58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H58" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5">
-        <v>2005325467</v>
-      </c>
-      <c r="B59" s="5">
-        <v>302159022</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>29</v>
-      </c>
-      <c r="H59" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5">
-        <v>2005325468</v>
-      </c>
-      <c r="B60" s="5">
-        <v>302159023</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>29</v>
-      </c>
-      <c r="H60" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="5">
-        <v>2005325469</v>
-      </c>
-      <c r="B61" s="5">
-        <v>302159024</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H61" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="5">
-        <v>2005325470</v>
-      </c>
-      <c r="B62" s="5">
-        <v>302159025</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
-        <v>29</v>
-      </c>
-      <c r="H62" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B62">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="B2:B55">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:C53">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C61">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2204,10 +2031,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Correccion de errores de carga a tabla salidas temp
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\LOGI\Carga Masiva\Masivo Inventario Alistamiento\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -30,7 +25,7 @@
     <author>Andres</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +395,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -530,9 +525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,11 +535,14 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -555,16 +550,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -740,16 +725,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -775,156 +750,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -984,7 +809,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1019,7 +844,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1231,8 +1056,8 @@
   <dimension ref="A1:U74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O71" sqref="O71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,68 +1081,68 @@
     <col min="21" max="21" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1352,6 +1177,9 @@
       <c r="M2" s="3">
         <v>0</v>
       </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
       <c r="Q2" t="s">
         <v>91</v>
       </c>
@@ -1359,11 +1187,11 @@
         <v>0</v>
       </c>
       <c r="T2" s="3">
-        <f>VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="T2:T33" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="U2" s="3">
-        <f>VLOOKUP(F2,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="U2:U33" si="1">VLOOKUP(F2,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -1408,11 +1236,11 @@
         <v>0</v>
       </c>
       <c r="T3" s="3">
-        <f>VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U3" s="3">
-        <f>VLOOKUP(F3,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1457,11 +1285,11 @@
         <v>0</v>
       </c>
       <c r="T4" s="3">
-        <f>VLOOKUP(E4,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="U4" s="3">
-        <f>VLOOKUP(F4,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1506,11 +1334,11 @@
         <v>0</v>
       </c>
       <c r="T5" s="3">
-        <f>VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U5" s="3">
-        <f>VLOOKUP(F5,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1555,11 +1383,11 @@
         <v>0</v>
       </c>
       <c r="T6" s="3">
-        <f>VLOOKUP(E6,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U6" s="3">
-        <f>VLOOKUP(F6,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1604,11 +1432,11 @@
         <v>0</v>
       </c>
       <c r="T7" s="3">
-        <f>VLOOKUP(E7,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U7" s="3">
-        <f>VLOOKUP(F7,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1653,11 +1481,11 @@
         <v>0</v>
       </c>
       <c r="T8" s="3">
-        <f>VLOOKUP(E8,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U8" s="3">
-        <f>VLOOKUP(F8,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1702,11 +1530,11 @@
         <v>0</v>
       </c>
       <c r="T9" s="3">
-        <f>VLOOKUP(E9,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U9" s="3">
-        <f>VLOOKUP(F9,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1751,11 +1579,11 @@
         <v>0</v>
       </c>
       <c r="T10" s="3">
-        <f>VLOOKUP(E10,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U10" s="3">
-        <f>VLOOKUP(F10,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1800,11 +1628,11 @@
         <v>0</v>
       </c>
       <c r="T11" s="3">
-        <f>VLOOKUP(E11,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U11" s="3">
-        <f>VLOOKUP(F11,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1849,11 +1677,11 @@
         <v>0</v>
       </c>
       <c r="T12" s="3">
-        <f>VLOOKUP(E12,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U12" s="3">
-        <f>VLOOKUP(F12,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1898,11 +1726,11 @@
         <v>0</v>
       </c>
       <c r="T13" s="3">
-        <f>VLOOKUP(E13,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="U13" s="3">
-        <f>VLOOKUP(F13,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1947,11 +1775,11 @@
         <v>0</v>
       </c>
       <c r="T14" s="3">
-        <f>VLOOKUP(E14,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U14" s="3">
-        <f>VLOOKUP(F14,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1996,11 +1824,11 @@
         <v>0</v>
       </c>
       <c r="T15" s="3">
-        <f>VLOOKUP(E15,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U15" s="3">
-        <f>VLOOKUP(F15,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2045,11 +1873,11 @@
         <v>0</v>
       </c>
       <c r="T16" s="3">
-        <f>VLOOKUP(E16,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U16" s="3">
-        <f>VLOOKUP(F16,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2094,11 +1922,11 @@
         <v>0</v>
       </c>
       <c r="T17" s="3">
-        <f>VLOOKUP(E17,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U17" s="3">
-        <f>VLOOKUP(F17,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2143,11 +1971,11 @@
         <v>0</v>
       </c>
       <c r="T18" s="3">
-        <f>VLOOKUP(E18,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U18" s="3">
-        <f>VLOOKUP(F18,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2192,11 +2020,11 @@
         <v>0</v>
       </c>
       <c r="T19" s="3">
-        <f>VLOOKUP(E19,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U19" s="3">
-        <f>VLOOKUP(F19,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2241,11 +2069,11 @@
         <v>0</v>
       </c>
       <c r="T20" s="3">
-        <f>VLOOKUP(E20,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U20" s="3">
-        <f>VLOOKUP(F20,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2290,11 +2118,11 @@
         <v>0</v>
       </c>
       <c r="T21" s="3">
-        <f>VLOOKUP(E21,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U21" s="3">
-        <f>VLOOKUP(F21,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2339,11 +2167,11 @@
         <v>0</v>
       </c>
       <c r="T22" s="3">
-        <f>VLOOKUP(E22,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="U22" s="3">
-        <f>VLOOKUP(F22,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2388,11 +2216,11 @@
         <v>0</v>
       </c>
       <c r="T23" s="3">
-        <f>VLOOKUP(E23,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U23" s="3">
-        <f>VLOOKUP(F23,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2437,11 +2265,11 @@
         <v>0</v>
       </c>
       <c r="T24" s="3">
-        <f>VLOOKUP(E24,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U24" s="3">
-        <f>VLOOKUP(F24,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2486,11 +2314,11 @@
         <v>0</v>
       </c>
       <c r="T25" s="3">
-        <f>VLOOKUP(E25,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U25" s="3">
-        <f>VLOOKUP(F25,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2550,11 +2378,11 @@
         <v>0</v>
       </c>
       <c r="T26" s="3">
-        <f>VLOOKUP(E26,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U26" s="3">
-        <f>VLOOKUP(F26,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2614,11 +2442,11 @@
         <v>0</v>
       </c>
       <c r="T27" s="3">
-        <f>VLOOKUP(E27,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U27" s="3">
-        <f>VLOOKUP(F27,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2678,11 +2506,11 @@
         <v>0</v>
       </c>
       <c r="T28" s="3">
-        <f>VLOOKUP(E28,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U28" s="3">
-        <f>VLOOKUP(F28,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2742,11 +2570,11 @@
         <v>0</v>
       </c>
       <c r="T29" s="3">
-        <f>VLOOKUP(E29,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U29" s="3">
-        <f>VLOOKUP(F29,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2806,11 +2634,11 @@
         <v>0</v>
       </c>
       <c r="T30" s="3">
-        <f>VLOOKUP(E30,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U30" s="3">
-        <f>VLOOKUP(F30,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2870,11 +2698,11 @@
         <v>0</v>
       </c>
       <c r="T31" s="3">
-        <f>VLOOKUP(E31,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U31" s="3">
-        <f>VLOOKUP(F31,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2934,11 +2762,11 @@
         <v>0</v>
       </c>
       <c r="T32" s="3">
-        <f>VLOOKUP(E32,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U32" s="3">
-        <f>VLOOKUP(F32,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2998,11 +2826,11 @@
         <v>0</v>
       </c>
       <c r="T33" s="3">
-        <f>VLOOKUP(E33,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="U33" s="3">
-        <f>VLOOKUP(F33,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3062,11 +2890,11 @@
         <v>0</v>
       </c>
       <c r="T34" s="3">
-        <f>VLOOKUP(E34,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="T34:T65" si="2">VLOOKUP(E34,T_OPERADORES,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="U34" s="3">
-        <f>VLOOKUP(F34,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="U34:U65" si="3">VLOOKUP(F34,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -3126,11 +2954,11 @@
         <v>0</v>
       </c>
       <c r="T35" s="3">
-        <f>VLOOKUP(E35,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="U35" s="3">
-        <f>VLOOKUP(F35,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3190,11 +3018,11 @@
         <v>0</v>
       </c>
       <c r="T36" s="3">
-        <f>VLOOKUP(E36,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="U36" s="3">
-        <f>VLOOKUP(F36,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3254,11 +3082,11 @@
         <v>0</v>
       </c>
       <c r="T37" s="3">
-        <f>VLOOKUP(E37,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="U37" s="3">
-        <f>VLOOKUP(F37,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3318,11 +3146,11 @@
         <v>0</v>
       </c>
       <c r="T38" s="3">
-        <f>VLOOKUP(E38,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="U38" s="3">
-        <f>VLOOKUP(F38,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3369,11 +3197,11 @@
         <v>0</v>
       </c>
       <c r="T39" s="3">
-        <f>VLOOKUP(E39,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="U39" s="3">
-        <f>VLOOKUP(F39,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3419,11 +3247,11 @@
         <v>0</v>
       </c>
       <c r="T40" s="3">
-        <f>VLOOKUP(E40,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U40" s="3">
-        <f>VLOOKUP(F40,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3469,11 +3297,11 @@
         <v>0</v>
       </c>
       <c r="T41" s="3">
-        <f>VLOOKUP(E41,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U41" s="3">
-        <f>VLOOKUP(F41,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3519,11 +3347,11 @@
         <v>0</v>
       </c>
       <c r="T42" s="3">
-        <f>VLOOKUP(E42,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U42" s="3">
-        <f>VLOOKUP(F42,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3568,11 +3396,11 @@
         <v>0</v>
       </c>
       <c r="T43" s="3">
-        <f>VLOOKUP(E43,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U43" s="3">
-        <f>VLOOKUP(F43,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3617,11 +3445,11 @@
         <v>0</v>
       </c>
       <c r="T44" s="3">
-        <f>VLOOKUP(E44,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U44" s="3">
-        <f>VLOOKUP(F44,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3666,11 +3494,11 @@
         <v>0</v>
       </c>
       <c r="T45" s="3">
-        <f>VLOOKUP(E45,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U45" s="3">
-        <f>VLOOKUP(F45,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3715,11 +3543,11 @@
         <v>0</v>
       </c>
       <c r="T46" s="3">
-        <f>VLOOKUP(E46,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U46" s="3">
-        <f>VLOOKUP(F46,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3764,11 +3592,11 @@
         <v>0</v>
       </c>
       <c r="T47" s="3">
-        <f>VLOOKUP(E47,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U47" s="3">
-        <f>VLOOKUP(F47,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3813,11 +3641,11 @@
         <v>0</v>
       </c>
       <c r="T48" s="3">
-        <f>VLOOKUP(E48,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="U48" s="3">
-        <f>VLOOKUP(F48,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3862,11 +3690,11 @@
         <v>0</v>
       </c>
       <c r="T49" s="3">
-        <f>VLOOKUP(E49,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U49" s="3">
-        <f>VLOOKUP(F49,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3911,11 +3739,11 @@
         <v>0</v>
       </c>
       <c r="T50" s="3">
-        <f>VLOOKUP(E50,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U50" s="3">
-        <f>VLOOKUP(F50,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3960,11 +3788,11 @@
         <v>0</v>
       </c>
       <c r="T51" s="3">
-        <f>VLOOKUP(E51,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U51" s="3">
-        <f>VLOOKUP(F51,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4009,11 +3837,11 @@
         <v>0</v>
       </c>
       <c r="T52" s="3">
-        <f>VLOOKUP(E52,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U52" s="3">
-        <f>VLOOKUP(F52,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4058,11 +3886,11 @@
         <v>0</v>
       </c>
       <c r="T53" s="3">
-        <f>VLOOKUP(E53,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U53" s="3">
-        <f>VLOOKUP(F53,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4107,11 +3935,11 @@
         <v>0</v>
       </c>
       <c r="T54" s="3">
-        <f>VLOOKUP(E54,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U54" s="3">
-        <f>VLOOKUP(F54,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4156,11 +3984,11 @@
         <v>0</v>
       </c>
       <c r="T55" s="3">
-        <f>VLOOKUP(E55,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U55" s="3">
-        <f>VLOOKUP(F55,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4205,11 +4033,11 @@
         <v>0</v>
       </c>
       <c r="T56" s="3">
-        <f>VLOOKUP(E56,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U56" s="3">
-        <f>VLOOKUP(F56,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4254,11 +4082,11 @@
         <v>0</v>
       </c>
       <c r="T57" s="3">
-        <f>VLOOKUP(E57,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U57" s="3">
-        <f>VLOOKUP(F57,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4303,11 +4131,11 @@
         <v>0</v>
       </c>
       <c r="T58" s="3">
-        <f>VLOOKUP(E58,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U58" s="3">
-        <f>VLOOKUP(F58,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4352,11 +4180,11 @@
         <v>0</v>
       </c>
       <c r="T59" s="3">
-        <f>VLOOKUP(E59,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U59" s="3">
-        <f>VLOOKUP(F59,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4401,11 +4229,11 @@
         <v>0</v>
       </c>
       <c r="T60" s="3">
-        <f>VLOOKUP(E60,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U60" s="3">
-        <f>VLOOKUP(F60,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4450,11 +4278,11 @@
         <v>0</v>
       </c>
       <c r="T61" s="3">
-        <f>VLOOKUP(E61,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U61" s="3">
-        <f>VLOOKUP(F61,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4499,11 +4327,11 @@
         <v>0</v>
       </c>
       <c r="T62" s="3">
-        <f>VLOOKUP(E62,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U62" s="3">
-        <f>VLOOKUP(F62,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4548,11 +4376,11 @@
         <v>0</v>
       </c>
       <c r="T63" s="3">
-        <f>VLOOKUP(E63,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U63" s="3">
-        <f>VLOOKUP(F63,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4597,11 +4425,11 @@
         <v>0</v>
       </c>
       <c r="T64" s="3">
-        <f>VLOOKUP(E64,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U64" s="3">
-        <f>VLOOKUP(F64,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4646,11 +4474,11 @@
         <v>0</v>
       </c>
       <c r="T65" s="3">
-        <f>VLOOKUP(E65,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="U65" s="3">
-        <f>VLOOKUP(F65,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4695,11 +4523,11 @@
         <v>0</v>
       </c>
       <c r="T66" s="3">
-        <f>VLOOKUP(E66,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="T66:T74" si="4">VLOOKUP(E66,T_OPERADORES,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="U66" s="3">
-        <f>VLOOKUP(F66,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="U66:U74" si="5">VLOOKUP(F66,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -4744,11 +4572,11 @@
         <v>0</v>
       </c>
       <c r="T67" s="3">
-        <f>VLOOKUP(E67,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U67" s="3">
-        <f>VLOOKUP(F67,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4793,11 +4621,11 @@
         <v>0</v>
       </c>
       <c r="T68" s="3">
-        <f>VLOOKUP(E68,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U68" s="3">
-        <f>VLOOKUP(F68,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4842,11 +4670,11 @@
         <v>0</v>
       </c>
       <c r="T69" s="3">
-        <f>VLOOKUP(E69,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U69" s="3">
-        <f>VLOOKUP(F69,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4891,11 +4719,11 @@
         <v>0</v>
       </c>
       <c r="T70" s="3">
-        <f>VLOOKUP(E70,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U70" s="3">
-        <f>VLOOKUP(F70,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4940,11 +4768,11 @@
         <v>0</v>
       </c>
       <c r="T71" s="3">
-        <f>VLOOKUP(E71,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U71" s="3">
-        <f>VLOOKUP(F71,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4989,11 +4817,11 @@
         <v>0</v>
       </c>
       <c r="T72" s="3">
-        <f>VLOOKUP(E72,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U72" s="3">
-        <f>VLOOKUP(F72,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -5038,11 +4866,11 @@
         <v>0</v>
       </c>
       <c r="T73" s="3">
-        <f>VLOOKUP(E73,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="U73" s="3">
-        <f>VLOOKUP(F73,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -5087,77 +4915,77 @@
         <v>0</v>
       </c>
       <c r="T74" s="3">
-        <f>VLOOKUP(E74,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U74" s="3">
-        <f>VLOOKUP(F74,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="37" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="duplicateValues" dxfId="36" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B74">
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:C53">
-    <cfRule type="duplicateValues" dxfId="35" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="duplicateValues" dxfId="34" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C62 C64 C70 C75:C1048576">
-    <cfRule type="duplicateValues" dxfId="33" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C61">
-    <cfRule type="duplicateValues" dxfId="32" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="duplicateValues" dxfId="31" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="duplicateValues" dxfId="30" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="29" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="28" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C69">
-    <cfRule type="duplicateValues" dxfId="27" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C69">
-    <cfRule type="duplicateValues" dxfId="26" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="duplicateValues" dxfId="24" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71 C75:C1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5180,14 +5008,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Modificacion en carga de xlsx entradas de invntario add de campo costo unitario en producto
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\LOGI\Carga Masiva\Masivo Inventario Alistamiento\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -25,7 +30,7 @@
     <author>Andres</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="109">
   <si>
     <t>Guia</t>
   </si>
@@ -390,12 +395,51 @@
   </si>
   <si>
     <t>EMSG0002</t>
+  </si>
+  <si>
+    <t>ACS00428</t>
+  </si>
+  <si>
+    <t>065CS25126</t>
+  </si>
+  <si>
+    <t>XDSG0016</t>
+  </si>
+  <si>
+    <t>XDAP0001</t>
+  </si>
+  <si>
+    <t>ESXI0005</t>
+  </si>
+  <si>
+    <t>ACEC0010</t>
+  </si>
+  <si>
+    <t>FSSG0031</t>
+  </si>
+  <si>
+    <t>FXXI0022</t>
+  </si>
+  <si>
+    <t>FXXI0023</t>
+  </si>
+  <si>
+    <t>XDXI0009</t>
+  </si>
+  <si>
+    <t>EP-DA705BBEGWW</t>
+  </si>
+  <si>
+    <t>TA20MICRO-BLANCO</t>
+  </si>
+  <si>
+    <t>TA20USBC-BLANCO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -538,21 +582,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -725,6 +765,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -809,7 +859,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,7 +894,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1055,16 +1105,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="3" customWidth="1"/>
@@ -3161,8 +3211,8 @@
       <c r="B39" s="3">
         <v>302159002</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>8</v>
+      <c r="C39" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
@@ -3212,8 +3262,8 @@
       <c r="B40" s="3">
         <v>302159003</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>9</v>
+      <c r="C40" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>
@@ -3262,8 +3312,8 @@
       <c r="B41" s="3">
         <v>302159004</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>10</v>
+      <c r="C41" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="D41" s="3">
         <v>3</v>
@@ -3312,8 +3362,8 @@
       <c r="B42" s="3">
         <v>302159005</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>11</v>
+      <c r="C42" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="D42" s="3">
         <v>1</v>
@@ -3362,8 +3412,8 @@
       <c r="B43" s="3">
         <v>302159006</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>12</v>
+      <c r="C43" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
@@ -3411,8 +3461,8 @@
       <c r="B44" s="3">
         <v>302159007</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>13</v>
+      <c r="C44" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
@@ -3460,8 +3510,8 @@
       <c r="B45" s="3">
         <v>302159008</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>14</v>
+      <c r="C45" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="D45" s="3">
         <v>1</v>
@@ -3509,8 +3559,8 @@
       <c r="B46" s="3">
         <v>302159009</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>15</v>
+      <c r="C46" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="D46" s="3">
         <v>3</v>
@@ -3558,8 +3608,8 @@
       <c r="B47" s="3">
         <v>302159010</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>16</v>
+      <c r="C47" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
@@ -3607,8 +3657,8 @@
       <c r="B48" s="3">
         <v>302159011</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>17</v>
+      <c r="C48" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
@@ -3656,8 +3706,8 @@
       <c r="B49" s="3">
         <v>302159012</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>18</v>
+      <c r="C49" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
@@ -3705,8 +3755,8 @@
       <c r="B50" s="3">
         <v>302159013</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>19</v>
+      <c r="C50" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
@@ -3754,8 +3804,8 @@
       <c r="B51" s="3">
         <v>302159014</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>20</v>
+      <c r="C51" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="D51" s="3">
         <v>1</v>
@@ -3803,8 +3853,8 @@
       <c r="B52" s="3">
         <v>302159015</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>21</v>
+      <c r="C52" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="D52" s="3">
         <v>2</v>
@@ -4934,58 +4984,58 @@
     <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B74">
-    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:C53">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C62 C64 C70 C75:C1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
+  <conditionalFormatting sqref="C1:C38 C64 C70 C75:C1048576 C53:C62">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C61">
-    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C69">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C69">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C71 C75:C1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="C1:C38 C75:C1048576 C53:C71">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Control de creacion de os y registro en tabla salidas desde tabla salidas temp TERMINADO para el ingreso uno a uno con boton GO
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="120">
   <si>
     <t>Guia</t>
   </si>
@@ -279,12 +279,6 @@
     <t>CL 10 32 A 12</t>
   </si>
   <si>
-    <t>CR 19 A 90 12</t>
-  </si>
-  <si>
-    <t>CR 69 25 B 44 OFI 508</t>
-  </si>
-  <si>
     <t>CL 61 5 20</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>CR 8 15 43 PISO 13</t>
   </si>
   <si>
-    <t>CR 13 27 47 PISO 4</t>
-  </si>
-  <si>
     <t>ALEJANDRO  VALLEJO SEADE</t>
   </si>
   <si>
@@ -315,12 +306,6 @@
     <t>FELIPE AYERBE MUÑOZ</t>
   </si>
   <si>
-    <t>ALEJANDRO ALBAN</t>
-  </si>
-  <si>
-    <t>WILLIAM DARIO PARDO MORENO</t>
-  </si>
-  <si>
     <t>TATIANA GARCES</t>
   </si>
   <si>
@@ -339,9 +324,6 @@
     <t>DIEGO FERNANDO PRIETO RIVERA</t>
   </si>
   <si>
-    <t>ALVARO  JARAMILLO</t>
-  </si>
-  <si>
     <t>TIPO ENVIO</t>
   </si>
   <si>
@@ -456,7 +438,52 @@
     <t>LOGI</t>
   </si>
   <si>
-    <t>GLAP0001</t>
+    <t>CÉSAR AUGUSTO JARAMILLO RESTREPO</t>
+  </si>
+  <si>
+    <t>RUDOLF  HOMMES</t>
+  </si>
+  <si>
+    <t>OSCAR  SANTOS</t>
+  </si>
+  <si>
+    <t>CARLOS MARIO RESTREPO</t>
+  </si>
+  <si>
+    <t>LEON DARÍO URIBE MESA</t>
+  </si>
+  <si>
+    <t>LUZ ADRIANA OSORIO</t>
+  </si>
+  <si>
+    <t>MÓNICA  LONDOÑO</t>
+  </si>
+  <si>
+    <t>CAMILO  ROMERO</t>
+  </si>
+  <si>
+    <t>DG 115 A 70 C 75 PISO 5 PRESIDENCIA CLÍNICA SHAIO</t>
+  </si>
+  <si>
+    <t>CR 17 119 A 09</t>
+  </si>
+  <si>
+    <t>CL 17 N 6 53</t>
+  </si>
+  <si>
+    <t>CR 11 B 98 08 OF 505</t>
+  </si>
+  <si>
+    <t>CR 10 86 13 APTO 801</t>
+  </si>
+  <si>
+    <t>KM 1 VIA OCAÑA AGUACHICA CESAR</t>
+  </si>
+  <si>
+    <t>AV ENIDA CR 45 103 60 EDIFICIO DIREC TR PISO 8</t>
+  </si>
+  <si>
+    <t>AV CR 45 103 60 EDIFICIO DIREC TR PISO 8</t>
   </si>
 </sst>
 </file>
@@ -631,7 +658,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -639,6 +666,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -759,56 +816,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1142,11 +1149,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V75"/>
+  <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,10 +1195,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>5</v>
@@ -1200,43 +1207,43 @@
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="U1" s="9" t="s">
         <v>30</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1259,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1277,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1311,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1329,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -1363,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1381,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1415,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -1433,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S5" s="3">
         <v>0</v>
@@ -1467,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -1485,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S6" s="3">
         <v>0</v>
@@ -1519,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
@@ -1537,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S7" s="3">
         <v>0</v>
@@ -1571,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
@@ -1589,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S8" s="3">
         <v>0</v>
@@ -1623,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K9" s="3">
         <v>1</v>
@@ -1641,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S9" s="3">
         <v>0</v>
@@ -1675,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K10" s="3">
         <v>1</v>
@@ -1693,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S10" s="3">
         <v>0</v>
@@ -1727,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K11" s="3">
         <v>1</v>
@@ -1745,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S11" s="3">
         <v>0</v>
@@ -1779,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -1797,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S12" s="3">
         <v>0</v>
@@ -1831,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
@@ -1849,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S13" s="3">
         <v>0</v>
@@ -1883,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K14" s="3">
         <v>1</v>
@@ -1901,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S14" s="3">
         <v>0</v>
@@ -1935,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K15" s="3">
         <v>1</v>
@@ -1953,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S15" s="3">
         <v>0</v>
@@ -1987,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K16" s="3">
         <v>1</v>
@@ -2005,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S16" s="3">
         <v>0</v>
@@ -2039,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K17" s="3">
         <v>1</v>
@@ -2057,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S17" s="3">
         <v>0</v>
@@ -2091,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K18" s="3">
         <v>1</v>
@@ -2109,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S18" s="3">
         <v>0</v>
@@ -2143,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
@@ -2161,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S19" s="3">
         <v>0</v>
@@ -2195,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -2213,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S20" s="3">
         <v>0</v>
@@ -2247,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K21" s="3">
         <v>1</v>
@@ -2265,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S21" s="3">
         <v>0</v>
@@ -2299,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K22" s="3">
         <v>1</v>
@@ -2317,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S22" s="3">
         <v>0</v>
@@ -2351,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K23" s="3">
         <v>1</v>
@@ -2369,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S23" s="3">
         <v>0</v>
@@ -2403,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K24" s="3">
         <v>1</v>
@@ -2421,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S24" s="3">
         <v>0</v>
@@ -2455,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K25" s="3">
         <v>1</v>
@@ -2473,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S25" s="3">
         <v>0</v>
@@ -2501,19 +2508,19 @@
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="J26" s="3">
         <v>312685412</v>
@@ -2534,13 +2541,13 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q26" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S26" s="3">
         <v>0</v>
@@ -2568,19 +2575,19 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="J27" s="3">
         <v>310546987</v>
@@ -2601,13 +2608,13 @@
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S27" s="3">
         <v>0</v>
@@ -2635,19 +2642,19 @@
         <v>2</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="J28" s="3">
         <v>300452362</v>
@@ -2668,13 +2675,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S28" s="3">
         <v>0</v>
@@ -2702,19 +2709,19 @@
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="J29" s="3">
         <v>320412214</v>
@@ -2735,13 +2742,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S29" s="3">
         <v>0</v>
@@ -2769,22 +2776,22 @@
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="J30" s="3">
-        <v>301956332</v>
+        <v>320412214</v>
       </c>
       <c r="K30" s="3">
         <v>1</v>
@@ -2802,13 +2809,13 @@
         <v>0</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S30" s="3">
         <v>0</v>
@@ -2836,22 +2843,22 @@
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J31" s="3">
-        <v>302778899</v>
+        <v>320412214</v>
       </c>
       <c r="K31" s="3">
         <v>1</v>
@@ -2869,13 +2876,13 @@
         <v>0</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S31" s="3">
         <v>0</v>
@@ -2903,19 +2910,19 @@
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="J32" s="3">
         <v>304623212</v>
@@ -2936,13 +2943,13 @@
         <v>0</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S32" s="3">
         <v>0</v>
@@ -2970,19 +2977,19 @@
         <v>3</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="J33" s="3">
         <v>315452325</v>
@@ -3003,13 +3010,13 @@
         <v>0</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S33" s="3">
         <v>0</v>
@@ -3037,19 +3044,19 @@
         <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="J34" s="3">
         <v>300656332</v>
@@ -3070,13 +3077,13 @@
         <v>0</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S34" s="3">
         <v>0</v>
@@ -3104,19 +3111,19 @@
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="J35" s="3">
         <v>320421305</v>
@@ -3137,13 +3144,13 @@
         <v>0</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S35" s="3">
         <v>0</v>
@@ -3171,19 +3178,19 @@
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="J36" s="3">
         <v>300500213</v>
@@ -3204,13 +3211,13 @@
         <v>0</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S36" s="3">
         <v>0</v>
@@ -3238,19 +3245,19 @@
         <v>1</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="J37" s="3">
         <v>310963258</v>
@@ -3271,13 +3278,13 @@
         <v>0</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S37" s="3">
         <v>0</v>
@@ -3293,10 +3300,10 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>2005325446</v>
+        <v>2005325445</v>
       </c>
       <c r="B38" s="3">
-        <v>302159001</v>
+        <v>302159000</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>43</v>
@@ -3305,22 +3312,22 @@
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="J38" s="3">
-        <v>300412500</v>
+        <v>310963258</v>
       </c>
       <c r="K38" s="3">
         <v>1</v>
@@ -3338,13 +3345,13 @@
         <v>0</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S38" s="3">
         <v>0</v>
@@ -3366,7 +3373,7 @@
         <v>302159002</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
@@ -3378,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="3"/>
@@ -3398,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S39" s="3">
         <v>0</v>
@@ -3420,7 +3427,7 @@
         <v>302159003</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>
@@ -3432,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H40" s="5"/>
       <c r="K40" s="3">
@@ -3451,7 +3458,7 @@
         <v>0</v>
       </c>
       <c r="R40" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S40" s="3">
         <v>0</v>
@@ -3473,7 +3480,7 @@
         <v>302159004</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3">
         <v>3</v>
@@ -3485,9 +3492,9 @@
         <v>0</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H41" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="H41" s="3"/>
       <c r="K41" s="3">
         <v>1</v>
       </c>
@@ -3504,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S41" s="3">
         <v>0</v>
@@ -3526,7 +3533,7 @@
         <v>302159005</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3">
         <v>1</v>
@@ -3538,9 +3545,9 @@
         <v>0</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H42" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="H42" s="3"/>
       <c r="K42" s="3">
         <v>1</v>
       </c>
@@ -3557,7 +3564,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S42" s="3">
         <v>0</v>
@@ -3573,13 +3580,13 @@
     </row>
     <row r="43" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>2005325451</v>
+        <v>2005325450</v>
       </c>
       <c r="B43" s="3">
-        <v>302159006</v>
+        <v>302159005</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
@@ -3591,8 +3598,9 @@
         <v>0</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H43" s="3"/>
       <c r="K43" s="3">
         <v>1</v>
       </c>
@@ -3609,7 +3617,7 @@
         <v>0</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S43" s="3">
         <v>0</v>
@@ -3625,26 +3633,27 @@
     </row>
     <row r="44" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>2005325452</v>
+        <v>2005325450</v>
       </c>
       <c r="B44" s="3">
-        <v>302159007</v>
+        <v>302159005</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F44" s="3">
         <v>0</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H44" s="3"/>
       <c r="K44" s="3">
         <v>1</v>
       </c>
@@ -3661,14 +3670,14 @@
         <v>0</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S44" s="3">
         <v>0</v>
       </c>
       <c r="U44" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V44" s="3">
         <f t="shared" si="3"/>
@@ -3683,7 +3692,7 @@
         <v>302159008</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D45" s="3">
         <v>1</v>
@@ -3695,8 +3704,9 @@
         <v>0</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H45" s="3"/>
       <c r="K45" s="3">
         <v>1</v>
       </c>
@@ -3713,7 +3723,7 @@
         <v>0</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S45" s="3">
         <v>0</v>
@@ -3735,7 +3745,7 @@
         <v>302159009</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D46" s="3">
         <v>3</v>
@@ -3747,8 +3757,9 @@
         <v>0</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H46" s="3"/>
       <c r="K46" s="3">
         <v>1</v>
       </c>
@@ -3765,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S46" s="3">
         <v>0</v>
@@ -3787,7 +3798,7 @@
         <v>302159010</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
@@ -3799,8 +3810,9 @@
         <v>0</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H47" s="3"/>
       <c r="K47" s="3">
         <v>1</v>
       </c>
@@ -3817,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S47" s="3">
         <v>0</v>
@@ -3839,7 +3851,7 @@
         <v>302159011</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
@@ -3851,8 +3863,9 @@
         <v>0</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H48" s="3"/>
       <c r="K48" s="3">
         <v>1</v>
       </c>
@@ -3869,7 +3882,7 @@
         <v>0</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S48" s="3">
         <v>0</v>
@@ -3891,7 +3904,7 @@
         <v>302159012</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
@@ -3903,8 +3916,9 @@
         <v>0</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H49" s="3"/>
       <c r="K49" s="3">
         <v>1</v>
       </c>
@@ -3921,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S49" s="3">
         <v>0</v>
@@ -3943,7 +3957,7 @@
         <v>302159013</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
@@ -3955,8 +3969,9 @@
         <v>0</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H50" s="3"/>
       <c r="K50" s="3">
         <v>1</v>
       </c>
@@ -3973,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S50" s="3">
         <v>0</v>
@@ -3995,7 +4010,7 @@
         <v>302159014</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D51" s="3">
         <v>1</v>
@@ -4007,8 +4022,9 @@
         <v>0</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H51" s="3"/>
       <c r="K51" s="3">
         <v>1</v>
       </c>
@@ -4025,7 +4041,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S51" s="3">
         <v>0</v>
@@ -4047,7 +4063,7 @@
         <v>302159015</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D52" s="3">
         <v>2</v>
@@ -4059,8 +4075,9 @@
         <v>0</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H52" s="3"/>
       <c r="K52" s="3">
         <v>1</v>
       </c>
@@ -4077,7 +4094,7 @@
         <v>0</v>
       </c>
       <c r="R52" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S52" s="3">
         <v>0</v>
@@ -4111,8 +4128,9 @@
         <v>0</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H53" s="3"/>
       <c r="K53" s="3">
         <v>1</v>
       </c>
@@ -4129,7 +4147,7 @@
         <v>0</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S53" s="3">
         <v>0</v>
@@ -4163,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K54" s="3">
         <v>1</v>
@@ -4181,7 +4199,7 @@
         <v>0</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S54" s="3">
         <v>0</v>
@@ -4215,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K55" s="3">
         <v>1</v>
@@ -4233,7 +4251,7 @@
         <v>0</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S55" s="3">
         <v>0</v>
@@ -4267,7 +4285,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K56" s="3">
         <v>1</v>
@@ -4285,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S56" s="3">
         <v>0</v>
@@ -4319,7 +4337,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K57" s="3">
         <v>1</v>
@@ -4337,7 +4355,7 @@
         <v>0</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S57" s="3">
         <v>0</v>
@@ -4371,7 +4389,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K58" s="3">
         <v>1</v>
@@ -4389,7 +4407,7 @@
         <v>0</v>
       </c>
       <c r="R58" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S58" s="3">
         <v>0</v>
@@ -4423,7 +4441,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K59" s="3">
         <v>1</v>
@@ -4441,7 +4459,7 @@
         <v>0</v>
       </c>
       <c r="R59" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S59" s="3">
         <v>0</v>
@@ -4468,14 +4486,23 @@
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="E60" t="s">
-        <v>29</v>
+      <c r="E60" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J60" s="3">
+        <v>315952014</v>
       </c>
       <c r="K60" s="3">
         <v>1</v>
@@ -4493,14 +4520,14 @@
         <v>0</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S60" s="3">
         <v>0</v>
       </c>
       <c r="U60" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V60" s="3">
         <f t="shared" si="3"/>
@@ -4520,14 +4547,23 @@
       <c r="D61">
         <v>1</v>
       </c>
-      <c r="E61" t="s">
-        <v>29</v>
+      <c r="E61" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F61" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J61" s="3">
+        <v>315746952</v>
       </c>
       <c r="K61" s="3">
         <v>1</v>
@@ -4545,14 +4581,14 @@
         <v>0</v>
       </c>
       <c r="R61" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S61" s="3">
         <v>0</v>
       </c>
       <c r="U61" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V61" s="3">
         <f t="shared" si="3"/>
@@ -4572,14 +4608,23 @@
       <c r="D62">
         <v>1</v>
       </c>
-      <c r="E62" t="s">
-        <v>29</v>
+      <c r="E62" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F62" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J62" s="3">
+        <v>300852165</v>
       </c>
       <c r="K62" s="3">
         <v>1</v>
@@ -4597,14 +4642,14 @@
         <v>0</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S62" s="3">
         <v>0</v>
       </c>
       <c r="U62" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V62" s="3">
         <f t="shared" si="3"/>
@@ -4619,19 +4664,28 @@
         <v>302159026</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
-      <c r="E63" t="s">
-        <v>31</v>
+      <c r="E63" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F63" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J63" s="3">
+        <v>302654872</v>
       </c>
       <c r="K63" s="3">
         <v>1</v>
@@ -4649,14 +4703,14 @@
         <v>0</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S63" s="3">
         <v>0</v>
       </c>
       <c r="U63" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V63" s="3">
         <f t="shared" si="3"/>
@@ -4676,14 +4730,23 @@
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64" t="s">
-        <v>31</v>
+      <c r="E64" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F64" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J64" s="3">
+        <v>302654872</v>
       </c>
       <c r="K64" s="3">
         <v>1</v>
@@ -4701,14 +4764,14 @@
         <v>0</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S64" s="3">
         <v>0</v>
       </c>
       <c r="U64" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V64" s="3">
         <f t="shared" si="3"/>
@@ -4723,19 +4786,28 @@
         <v>302159026</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
-      <c r="E65" t="s">
-        <v>31</v>
+      <c r="E65" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F65" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J65" s="3">
+        <v>302654872</v>
       </c>
       <c r="K65" s="3">
         <v>1</v>
@@ -4753,14 +4825,14 @@
         <v>0</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S65" s="3">
         <v>0</v>
       </c>
       <c r="U65" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V65" s="3">
         <f t="shared" si="3"/>
@@ -4780,14 +4852,23 @@
       <c r="D66">
         <v>2</v>
       </c>
-      <c r="E66" t="s">
-        <v>31</v>
+      <c r="E66" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F66" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J66" s="3">
+        <v>316803001</v>
       </c>
       <c r="K66" s="3">
         <v>1</v>
@@ -4805,17 +4886,17 @@
         <v>0</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S66" s="3">
         <v>0</v>
       </c>
       <c r="U66" s="3">
-        <f t="shared" ref="U66:U75" si="4">VLOOKUP(E66,T_OPERADORES,2,FALSE)</f>
-        <v>2</v>
+        <f t="shared" ref="U66:U73" si="4">VLOOKUP(E66,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="V66" s="3">
-        <f t="shared" ref="V66:V75" si="5">VLOOKUP(G66,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="V66:V73" si="5">VLOOKUP(G66,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -4832,14 +4913,23 @@
       <c r="D67">
         <v>2</v>
       </c>
-      <c r="E67" t="s">
-        <v>31</v>
+      <c r="E67" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F67" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J67" s="3">
+        <v>320464331</v>
       </c>
       <c r="K67" s="3">
         <v>1</v>
@@ -4857,14 +4947,14 @@
         <v>0</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S67" s="3">
         <v>0</v>
       </c>
       <c r="U67" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V67" s="3">
         <f t="shared" si="5"/>
@@ -4879,19 +4969,28 @@
         <v>302159031</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
-      <c r="E68" t="s">
-        <v>29</v>
+      <c r="E68" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F68" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J68" s="3">
+        <v>321932510</v>
       </c>
       <c r="K68" s="3">
         <v>1</v>
@@ -4909,14 +5008,14 @@
         <v>0</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S68" s="3">
         <v>0</v>
       </c>
       <c r="U68" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V68" s="3">
         <f t="shared" si="5"/>
@@ -4936,14 +5035,23 @@
       <c r="D69">
         <v>1</v>
       </c>
-      <c r="E69" t="s">
-        <v>29</v>
+      <c r="E69" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F69" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J69" s="3">
+        <v>300211548</v>
       </c>
       <c r="K69" s="3">
         <v>1</v>
@@ -4961,14 +5069,14 @@
         <v>0</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S69" s="3">
         <v>0</v>
       </c>
       <c r="U69" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V69" s="3">
         <f t="shared" si="5"/>
@@ -4995,8 +5103,9 @@
         <v>0</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H70" s="3"/>
       <c r="K70" s="3">
         <v>1</v>
       </c>
@@ -5013,7 +5122,7 @@
         <v>0</v>
       </c>
       <c r="R70" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S70" s="3">
         <v>0</v>
@@ -5035,7 +5144,7 @@
         <v>302159034</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -5047,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K71" s="3">
         <v>1</v>
@@ -5065,7 +5174,7 @@
         <v>0</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S71" s="3">
         <v>0</v>
@@ -5087,7 +5196,7 @@
         <v>302159035</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -5099,7 +5208,7 @@
         <v>0</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K72" s="3">
         <v>1</v>
@@ -5117,7 +5226,7 @@
         <v>0</v>
       </c>
       <c r="R72" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S72" s="3">
         <v>0</v>
@@ -5151,7 +5260,7 @@
         <v>0</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K73" s="3">
         <v>1</v>
@@ -5169,7 +5278,7 @@
         <v>0</v>
       </c>
       <c r="R73" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S73" s="3">
         <v>0</v>
@@ -5183,127 +5292,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3">
-        <v>302159037</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74">
-        <v>3</v>
-      </c>
-      <c r="E74" t="s">
-        <v>109</v>
-      </c>
-      <c r="F74" s="3">
-        <v>1</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K74" s="3">
-        <v>1</v>
-      </c>
-      <c r="L74" s="3">
-        <v>0</v>
-      </c>
-      <c r="M74" s="3">
-        <v>0</v>
-      </c>
-      <c r="N74" s="3">
-        <v>0</v>
-      </c>
-      <c r="O74" s="3">
-        <v>0</v>
-      </c>
-      <c r="R74" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="S74" s="3">
-        <v>0</v>
-      </c>
-      <c r="U74" s="3">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="V74" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3">
-        <v>302159037</v>
-      </c>
-      <c r="C75" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75" t="s">
-        <v>109</v>
-      </c>
-      <c r="F75" s="3">
-        <v>1</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K75">
-        <v>1</v>
-      </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-      <c r="M75">
-        <v>0</v>
-      </c>
-      <c r="N75">
-        <v>0</v>
-      </c>
-      <c r="O75">
-        <v>0</v>
-      </c>
-      <c r="R75" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="S75">
-        <v>0</v>
-      </c>
-      <c r="U75" s="3">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="V75" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B75">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C38 C64 C70 C75:C1048576 C53:C62">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C61">
     <cfRule type="duplicateValues" dxfId="13" priority="14"/>
@@ -5335,17 +5338,17 @@
   <conditionalFormatting sqref="C71">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C38 C75:C1048576 C53:C71">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="B2:B73">
+    <cfRule type="duplicateValues" dxfId="3" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="C1:C38 C64 C70 C74:C1048576 C53:C62">
+    <cfRule type="duplicateValues" dxfId="2" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="C1:C38 C74:C1048576 C53:C71">
+    <cfRule type="duplicateValues" dxfId="1" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C72:C74">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C72:C73">
+    <cfRule type="duplicateValues" dxfId="0" priority="36"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5373,7 +5376,7 @@
       </c>
       <c r="B1" s="13"/>
       <c r="D1" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E1" s="13"/>
     </row>
@@ -5385,7 +5388,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -5399,7 +5402,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -5415,7 +5418,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -5431,7 +5434,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>

</xml_diff>

<commit_message>
vista de seguimiento de alistamiento terminado
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Guia</t>
   </si>
@@ -165,6 +165,24 @@
     <t>INTERAPIDISIMO</t>
   </si>
   <si>
+    <t>CR 11 93 53 OF 601</t>
+  </si>
+  <si>
+    <t>CL 116 N 7 15 INT 2 OFICINA 403</t>
+  </si>
+  <si>
+    <t>CL 10 32 A 12</t>
+  </si>
+  <si>
+    <t>ALEJANDRO  VALLEJO SEADE</t>
+  </si>
+  <si>
+    <t>LUIS FERNANDO VALLEJO GUTIERREZ</t>
+  </si>
+  <si>
+    <t>FELIPE AYERBE MUÑOZ</t>
+  </si>
+  <si>
     <t>TIPO ENVIO</t>
   </si>
   <si>
@@ -210,6 +228,12 @@
     <t>Cantidad Envios</t>
   </si>
   <si>
+    <t>BOGOTA</t>
+  </si>
+  <si>
+    <t>CUNDINAMARCA</t>
+  </si>
+  <si>
     <t>Accesorios Celular</t>
   </si>
   <si>
@@ -222,19 +246,13 @@
     <t>LOGI</t>
   </si>
   <si>
-    <t>EP-DA705BWEGWW</t>
-  </si>
-  <si>
-    <t>571CS21683</t>
-  </si>
-  <si>
-    <t>587CS22051</t>
-  </si>
-  <si>
-    <t>565CS20828</t>
-  </si>
-  <si>
-    <t>042CS20511</t>
+    <t>TA50-BLANCO</t>
+  </si>
+  <si>
+    <t>EP-DG950CBE-BULK</t>
+  </si>
+  <si>
+    <t>EF-ZG988CBEGUS</t>
   </si>
 </sst>
 </file>
@@ -368,10 +386,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,7 +410,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -402,16 +418,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -745,11 +751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,364 +765,387 @@
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="3"/>
-    <col min="22" max="22" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="1"/>
+    <col min="22" max="22" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="8" t="s">
+      <c r="S1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="8" t="s">
-        <v>26</v>
+      <c r="V1" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>7006521444</v>
-      </c>
-      <c r="B2" s="3">
-        <v>600008544</v>
+      <c r="A2" s="1">
+        <v>4200065842</v>
+      </c>
+      <c r="B2" s="1">
+        <v>999000231</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2">
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1">
+        <v>312685412</v>
+      </c>
+      <c r="K2" s="1">
         <v>1</v>
       </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="3">
-        <f t="shared" ref="U2:U6" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="V2" s="3">
-        <f t="shared" ref="V2:V6" si="1">VLOOKUP(G2,T_TIPO_ENVIO,2,FALSE)</f>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <f t="shared" ref="U2:U4" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="V2" s="1">
+        <f t="shared" ref="V2:V4" si="1">VLOOKUP(G2,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>7006521444</v>
-      </c>
-      <c r="B3" s="3">
-        <v>600008544</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
+      <c r="A3" s="1">
+        <v>4200065842</v>
+      </c>
+      <c r="B3" s="1">
+        <v>999000231</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3">
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>310546987</v>
+      </c>
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="U3" s="3">
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V3" s="3">
+        <v>4</v>
+      </c>
+      <c r="V3" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>7001254889</v>
+        <v>4200065842</v>
       </c>
       <c r="B4" s="1">
-        <v>600012111</v>
+        <v>999000231</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1">
+        <v>320412214</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="V4" s="3">
+        <v>4</v>
+      </c>
+      <c r="V4" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>8210211111</v>
-      </c>
-      <c r="B5" s="1">
-        <v>822223333</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V5" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>8210211111</v>
-      </c>
-      <c r="B6" s="3">
-        <v>822223333</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V6" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="3" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C6">
-    <cfRule type="duplicateValues" dxfId="1" priority="51"/>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="duplicateValues" dxfId="1" priority="87"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="0" priority="52"/>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="duplicateValues" dxfId="0" priority="89"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1129,7 +1158,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,14 +1168,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="D1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1155,10 +1184,10 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1166,13 +1195,13 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1180,15 +1209,15 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1196,15 +1225,15 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion de cierre de sesiones al culminar alistamiento
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="136">
   <si>
     <t>Guia</t>
   </si>
@@ -153,12 +153,6 @@
     <t>XDAP0003</t>
   </si>
   <si>
-    <t>XMAP0006</t>
-  </si>
-  <si>
-    <t>FUAP0001</t>
-  </si>
-  <si>
     <t>IGSG0011</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>FUSG0049</t>
   </si>
   <si>
-    <t>FUSG0050</t>
-  </si>
-  <si>
     <t>XDSG0029</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>FUSG0008</t>
   </si>
   <si>
-    <t>FUSG0014</t>
-  </si>
-  <si>
     <t>XDSG0001</t>
   </si>
   <si>
@@ -279,9 +267,6 @@
     <t>CL 10 32 A 12</t>
   </si>
   <si>
-    <t>CL 61 5 20</t>
-  </si>
-  <si>
     <t>CR 7 A 140 08 MONTELOMA 9 ATO 101</t>
   </si>
   <si>
@@ -306,9 +291,6 @@
     <t>FELIPE AYERBE MUÑOZ</t>
   </si>
   <si>
-    <t>TATIANA GARCES</t>
-  </si>
-  <si>
     <t>PABLO BICKENBACH</t>
   </si>
   <si>
@@ -393,9 +375,6 @@
     <t>ACS00428</t>
   </si>
   <si>
-    <t>065CS25126</t>
-  </si>
-  <si>
     <t>XDSG0016</t>
   </si>
   <si>
@@ -408,12 +387,6 @@
     <t>ACEC0010</t>
   </si>
   <si>
-    <t>FSSG0031</t>
-  </si>
-  <si>
-    <t>FXXI0022</t>
-  </si>
-  <si>
     <t>FXXI0023</t>
   </si>
   <si>
@@ -423,12 +396,6 @@
     <t>EP-DA705BBEGWW</t>
   </si>
   <si>
-    <t>TA20MICRO-BLANCO</t>
-  </si>
-  <si>
-    <t>TA20USBC-BLANCO</t>
-  </si>
-  <si>
     <t>MASLOGISTICA</t>
   </si>
   <si>
@@ -484,13 +451,94 @@
   </si>
   <si>
     <t>AV CR 45 103 60 EDIFICIO DIREC TR PISO 8</t>
+  </si>
+  <si>
+    <t>587CS22051</t>
+  </si>
+  <si>
+    <t>057CS22123</t>
+  </si>
+  <si>
+    <t>062CS24470</t>
+  </si>
+  <si>
+    <t>FUAP0006</t>
+  </si>
+  <si>
+    <t>ACCM0010</t>
+  </si>
+  <si>
+    <t>FSSG0058</t>
+  </si>
+  <si>
+    <t>EF-ZN980CBEGUS</t>
+  </si>
+  <si>
+    <t>DANIELA PULIDO</t>
+  </si>
+  <si>
+    <t>JULIANA RUIZ</t>
+  </si>
+  <si>
+    <t>HUGO FERNANDEZ</t>
+  </si>
+  <si>
+    <t>GISELA URREGO</t>
+  </si>
+  <si>
+    <t>YULI DANIELA DUARTE</t>
+  </si>
+  <si>
+    <t>NIDIA MARTIN</t>
+  </si>
+  <si>
+    <t>CALLE 5 # 25 - 37</t>
+  </si>
+  <si>
+    <t>CARRERA 45 # 85-32</t>
+  </si>
+  <si>
+    <t>CALLE 68 # 35-05</t>
+  </si>
+  <si>
+    <t>DG 39 # 45-45</t>
+  </si>
+  <si>
+    <t>CALLE 87 # 65-10</t>
+  </si>
+  <si>
+    <t>CARRERA 78 # 110-25</t>
+  </si>
+  <si>
+    <t>RAUL TRIANA</t>
+  </si>
+  <si>
+    <t>FERNANDO SANCHEZ</t>
+  </si>
+  <si>
+    <t>FEDERICO RAMIREZ</t>
+  </si>
+  <si>
+    <t>CL 85 # 45-25</t>
+  </si>
+  <si>
+    <t>CR 74 # 25 A - 32</t>
+  </si>
+  <si>
+    <t>CALLE 78 B # 42-21 Sur</t>
+  </si>
+  <si>
+    <t>ADAP0024</t>
+  </si>
+  <si>
+    <t>ACEC0018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,14 +548,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -631,34 +671,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -691,11 +749,151 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1149,16 +1347,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V73"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P69" sqref="P69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
@@ -1178,80 +1376,80 @@
     <col min="22" max="22" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="F1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2005325410</v>
+        <v>4000652003</v>
       </c>
       <c r="B2">
-        <v>302158965</v>
+        <v>300098765</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -1260,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1284,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1300,10 +1498,10 @@
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2005325411</v>
+        <v>5006500254</v>
       </c>
       <c r="B3" s="1">
-        <v>302158966</v>
+        <v>300098764</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -1311,14 +1509,14 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1336,14 +1534,14 @@
         <v>0</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="U3" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V3" s="3">
         <f t="shared" si="1"/>
@@ -1352,10 +1550,10 @@
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2005325412</v>
-      </c>
-      <c r="B4" s="1">
-        <v>302158967</v>
+        <v>5006523145</v>
+      </c>
+      <c r="B4" s="3">
+        <v>300098763</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1364,13 +1562,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1388,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1404,25 +1602,25 @@
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2005325413</v>
-      </c>
-      <c r="B5" s="1">
-        <v>302158968</v>
+        <v>4005325413</v>
+      </c>
+      <c r="B5" s="3">
+        <v>300098762</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -1440,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S5" s="3">
         <v>0</v>
@@ -1456,25 +1654,25 @@
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>2005325413</v>
+        <v>4005325413</v>
       </c>
       <c r="B6" s="3">
-        <v>302158968</v>
+        <v>300098762</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -1492,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S6" s="3">
         <v>0</v>
@@ -1508,25 +1706,25 @@
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>2005325413</v>
+        <v>4005325413</v>
       </c>
       <c r="B7" s="3">
-        <v>302158968</v>
+        <v>300098762</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
@@ -1544,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S7" s="3">
         <v>0</v>
@@ -1560,25 +1758,25 @@
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>2005325416</v>
-      </c>
-      <c r="B8" s="1">
-        <v>302158971</v>
+        <v>5001236892</v>
+      </c>
+      <c r="B8" s="3">
+        <v>300098759</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>29</v>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
@@ -1596,14 +1794,14 @@
         <v>0</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S8" s="3">
         <v>0</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V8" s="3">
         <f t="shared" si="1"/>
@@ -1612,25 +1810,25 @@
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>2005325417</v>
-      </c>
-      <c r="B9" s="1">
-        <v>302158972</v>
+        <v>5001234567</v>
+      </c>
+      <c r="B9" s="3">
+        <v>300098758</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K9" s="3">
         <v>1</v>
@@ -1648,14 +1846,14 @@
         <v>0</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S9" s="3">
         <v>0</v>
       </c>
       <c r="U9" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V9" s="3">
         <f t="shared" si="1"/>
@@ -1663,26 +1861,26 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>2005325418</v>
-      </c>
-      <c r="B10" s="1">
-        <v>302158973</v>
+      <c r="A10" s="3">
+        <v>5001234569</v>
+      </c>
+      <c r="B10" s="3">
+        <v>300098757</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>29</v>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K10" s="3">
         <v>1</v>
@@ -1700,14 +1898,14 @@
         <v>0</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S10" s="3">
         <v>0</v>
       </c>
       <c r="U10" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V10" s="3">
         <f t="shared" si="1"/>
@@ -1715,26 +1913,26 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>2005325419</v>
-      </c>
-      <c r="B11" s="1">
-        <v>302158974</v>
+      <c r="A11" s="3">
+        <v>5001234569</v>
+      </c>
+      <c r="B11" s="3">
+        <v>300098757</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K11" s="3">
         <v>1</v>
@@ -1752,14 +1950,14 @@
         <v>0</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S11" s="3">
         <v>0</v>
       </c>
       <c r="U11" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V11" s="3">
         <f t="shared" si="1"/>
@@ -1767,26 +1965,26 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>2005325420</v>
-      </c>
-      <c r="B12" s="1">
-        <v>302158975</v>
+      <c r="A12" s="3">
+        <v>5001234569</v>
+      </c>
+      <c r="B12" s="3">
+        <v>300098757</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
-        <v>31</v>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -1804,14 +2002,14 @@
         <v>0</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S12" s="3">
         <v>0</v>
       </c>
       <c r="U12" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V12" s="3">
         <f t="shared" si="1"/>
@@ -1819,26 +2017,26 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>2005325421</v>
-      </c>
-      <c r="B13" s="1">
-        <v>302158976</v>
+      <c r="A13" s="3">
+        <v>5001234571</v>
+      </c>
+      <c r="B13" s="3">
+        <v>300098754</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F13" s="3">
         <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
@@ -1856,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S13" s="3">
         <v>0</v>
@@ -1871,26 +2069,26 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>2005325422</v>
-      </c>
-      <c r="B14" s="1">
-        <v>302158977</v>
+      <c r="A14" s="3">
+        <v>5001234572</v>
+      </c>
+      <c r="B14" s="3">
+        <v>300098753</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>31</v>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F14" s="3">
         <v>0</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K14" s="3">
         <v>1</v>
@@ -1908,14 +2106,14 @@
         <v>0</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S14" s="3">
         <v>0</v>
       </c>
       <c r="U14" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="1"/>
@@ -1924,25 +2122,25 @@
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>2005325423</v>
-      </c>
-      <c r="B15" s="1">
-        <v>302158978</v>
+        <v>4005325423</v>
+      </c>
+      <c r="B15" s="3">
+        <v>300098752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K15" s="3">
         <v>1</v>
@@ -1960,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S15" s="3">
         <v>0</v>
@@ -1975,26 +2173,26 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>2005325423</v>
-      </c>
-      <c r="B16" s="1">
-        <v>302158978</v>
+      <c r="A16" s="3">
+        <v>4005325423</v>
+      </c>
+      <c r="B16" s="3">
+        <v>300098752</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K16" s="3">
         <v>1</v>
@@ -2012,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S16" s="3">
         <v>0</v>
@@ -2028,25 +2226,25 @@
     </row>
     <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>2005325423</v>
+        <v>4005325423</v>
       </c>
       <c r="B17" s="3">
-        <v>302158978</v>
+        <v>300098752</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F17" s="3">
         <v>0</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K17" s="3">
         <v>1</v>
@@ -2064,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S17" s="3">
         <v>0</v>
@@ -2080,25 +2278,25 @@
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>2005325423</v>
+        <v>4005325423</v>
       </c>
       <c r="B18" s="3">
-        <v>302158978</v>
+        <v>300098752</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K18" s="3">
         <v>1</v>
@@ -2116,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S18" s="3">
         <v>0</v>
@@ -2132,25 +2330,25 @@
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>2005325427</v>
-      </c>
-      <c r="B19" s="1">
-        <v>302158982</v>
+        <v>2005005427</v>
+      </c>
+      <c r="B19" s="3">
+        <v>300098748</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K19" s="3">
         <v>1</v>
@@ -2168,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S19" s="3">
         <v>0</v>
@@ -2184,25 +2382,25 @@
     </row>
     <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>2005325428</v>
-      </c>
-      <c r="B20" s="1">
-        <v>302158983</v>
+        <v>2005303428</v>
+      </c>
+      <c r="B20" s="3">
+        <v>300098747</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -2220,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S20" s="3">
         <v>0</v>
@@ -2236,25 +2434,25 @@
     </row>
     <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>2005325429</v>
-      </c>
-      <c r="B21" s="1">
-        <v>302158984</v>
+        <v>2005025429</v>
+      </c>
+      <c r="B21" s="3">
+        <v>300098746</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F21" s="3">
         <v>0</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K21" s="3">
         <v>1</v>
@@ -2272,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S21" s="3">
         <v>0</v>
@@ -2287,26 +2485,26 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>2005325429</v>
-      </c>
-      <c r="B22" s="1">
-        <v>302158984</v>
+      <c r="A22" s="3">
+        <v>2005025429</v>
+      </c>
+      <c r="B22" s="3">
+        <v>300098746</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K22" s="3">
         <v>1</v>
@@ -2324,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S22" s="3">
         <v>0</v>
@@ -2340,25 +2538,25 @@
     </row>
     <row r="23" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>2005325431</v>
-      </c>
-      <c r="B23" s="1">
-        <v>302158986</v>
+        <v>4005325431</v>
+      </c>
+      <c r="B23" s="3">
+        <v>300098744</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K23" s="3">
         <v>1</v>
@@ -2376,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S23" s="3">
         <v>0</v>
@@ -2392,25 +2590,25 @@
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>2005325432</v>
-      </c>
-      <c r="B24" s="1">
-        <v>302158987</v>
+        <v>4005325432</v>
+      </c>
+      <c r="B24" s="3">
+        <v>300098743</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F24" s="3">
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K24" s="3">
         <v>1</v>
@@ -2428,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S24" s="3">
         <v>0</v>
@@ -2444,25 +2642,25 @@
     </row>
     <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>2005325433</v>
-      </c>
-      <c r="B25" s="1">
-        <v>302158988</v>
+        <v>4005325433</v>
+      </c>
+      <c r="B25" s="3">
+        <v>300098742</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K25" s="3">
         <v>1</v>
@@ -2480,7 +2678,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S25" s="3">
         <v>0</v>
@@ -2496,31 +2694,31 @@
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>2005325434</v>
+        <v>4005325434</v>
       </c>
       <c r="B26" s="3">
-        <v>302158989</v>
+        <v>300098741</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J26" s="3">
         <v>312685412</v>
@@ -2541,13 +2739,13 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S26" s="3">
         <v>0</v>
@@ -2563,31 +2761,31 @@
     </row>
     <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>2005325435</v>
+        <v>4005325435</v>
       </c>
       <c r="B27" s="3">
-        <v>302158990</v>
+        <v>300098740</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J27" s="3">
         <v>310546987</v>
@@ -2608,13 +2806,13 @@
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S27" s="3">
         <v>0</v>
@@ -2630,31 +2828,31 @@
     </row>
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>2005325436</v>
+        <v>4005325436</v>
       </c>
       <c r="B28" s="3">
-        <v>302158991</v>
+        <v>300098739</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J28" s="3">
         <v>300452362</v>
@@ -2675,13 +2873,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S28" s="3">
         <v>0</v>
@@ -2697,31 +2895,31 @@
     </row>
     <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>2005325437</v>
+        <v>90021</v>
       </c>
       <c r="B29" s="3">
-        <v>302158992</v>
+        <v>300098737</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J29" s="3">
         <v>320412214</v>
@@ -2742,13 +2940,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S29" s="3">
         <v>0</v>
@@ -2764,31 +2962,31 @@
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>2005325437</v>
+        <v>90021</v>
       </c>
       <c r="B30" s="3">
-        <v>302158992</v>
+        <v>300098737</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J30" s="3">
         <v>320412214</v>
@@ -2809,13 +3007,13 @@
         <v>0</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S30" s="3">
         <v>0</v>
@@ -2831,31 +3029,31 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>2005325437</v>
+        <v>90021</v>
       </c>
       <c r="B31" s="3">
-        <v>302158992</v>
+        <v>300098737</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J31" s="3">
         <v>320412214</v>
@@ -2876,13 +3074,13 @@
         <v>0</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S31" s="3">
         <v>0</v>
@@ -2898,31 +3096,31 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>2005325437</v>
+        <v>90021</v>
       </c>
       <c r="B32" s="3">
-        <v>302158992</v>
+        <v>300098737</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J32" s="3">
         <v>304623212</v>
@@ -2943,13 +3141,13 @@
         <v>0</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S32" s="3">
         <v>0</v>
@@ -2965,31 +3163,31 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>2005325441</v>
+        <v>7321005469</v>
       </c>
       <c r="B33" s="3">
-        <v>302158996</v>
+        <v>300098734</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J33" s="3">
         <v>315452325</v>
@@ -3010,13 +3208,13 @@
         <v>0</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S33" s="3">
         <v>0</v>
@@ -3032,31 +3230,31 @@
     </row>
     <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>2005325442</v>
+        <v>7321005468</v>
       </c>
       <c r="B34" s="3">
-        <v>302158997</v>
+        <v>300098733</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J34" s="3">
         <v>300656332</v>
@@ -3077,53 +3275,53 @@
         <v>0</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S34" s="3">
         <v>0</v>
       </c>
       <c r="U34" s="3">
-        <f t="shared" ref="U34:U65" si="2">VLOOKUP(E34,T_OPERADORES,2,FALSE)</f>
+        <f t="shared" ref="U34:U57" si="2">VLOOKUP(E34,T_OPERADORES,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="V34" s="3">
-        <f t="shared" ref="V34:V65" si="3">VLOOKUP(G34,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="V34:V57" si="3">VLOOKUP(G34,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>2005325443</v>
+        <v>7321005467</v>
       </c>
       <c r="B35" s="3">
-        <v>302158998</v>
+        <v>300098732</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J35" s="3">
         <v>320421305</v>
@@ -3144,13 +3342,13 @@
         <v>0</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S35" s="3">
         <v>0</v>
@@ -3166,31 +3364,31 @@
     </row>
     <row r="36" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>2005325444</v>
+        <v>7321005466</v>
       </c>
       <c r="B36" s="3">
-        <v>302158999</v>
+        <v>300098731</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J36" s="3">
         <v>300500213</v>
@@ -3211,13 +3409,13 @@
         <v>0</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S36" s="3">
         <v>0</v>
@@ -3233,31 +3431,31 @@
     </row>
     <row r="37" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>2005325445</v>
+        <v>8002455</v>
       </c>
       <c r="B37" s="3">
-        <v>302159000</v>
+        <v>300098730</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J37" s="3">
         <v>310963258</v>
@@ -3278,13 +3476,13 @@
         <v>0</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S37" s="3">
         <v>0</v>
@@ -3300,31 +3498,31 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>2005325445</v>
+        <v>8002455</v>
       </c>
       <c r="B38" s="3">
-        <v>302159000</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>43</v>
+        <v>300098730</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J38" s="3">
         <v>310963258</v>
@@ -3345,13 +3543,13 @@
         <v>0</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S38" s="3">
         <v>0</v>
@@ -3367,28 +3565,35 @@
     </row>
     <row r="39" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>2005325447</v>
+        <v>8300540022</v>
       </c>
       <c r="B39" s="3">
-        <v>302159002</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>88</v>
+        <v>300098727</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="F39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J39" s="3">
+        <v>320548652</v>
+      </c>
       <c r="K39" s="3">
         <v>1</v>
       </c>
@@ -3404,15 +3609,21 @@
       <c r="O39" s="3">
         <v>0</v>
       </c>
+      <c r="P39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R39" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S39" s="3">
         <v>0</v>
       </c>
       <c r="U39" s="3">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V39" s="3">
         <f t="shared" si="3"/>
@@ -3421,27 +3632,35 @@
     </row>
     <row r="40" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>2005325448</v>
+        <v>8300540022</v>
       </c>
       <c r="B40" s="3">
-        <v>302159003</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>88</v>
+        <v>300098727</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F40" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H40" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J40" s="3">
+        <v>301855422</v>
+      </c>
       <c r="K40" s="3">
         <v>1</v>
       </c>
@@ -3457,15 +3676,21 @@
       <c r="O40" s="3">
         <v>0</v>
       </c>
+      <c r="P40" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R40" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S40" s="3">
         <v>0</v>
       </c>
       <c r="U40" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V40" s="3">
         <f t="shared" si="3"/>
@@ -3474,27 +3699,35 @@
     </row>
     <row r="41" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>2005325449</v>
+        <v>654000021</v>
       </c>
       <c r="B41" s="3">
-        <v>302159004</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>89</v>
+        <v>300098726</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="D41" s="3">
         <v>3</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H41" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J41" s="3">
+        <v>320766322</v>
+      </c>
       <c r="K41" s="3">
         <v>1</v>
       </c>
@@ -3510,15 +3743,21 @@
       <c r="O41" s="3">
         <v>0</v>
       </c>
+      <c r="P41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R41" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S41" s="3">
         <v>0</v>
       </c>
       <c r="U41" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V41" s="3">
         <f t="shared" si="3"/>
@@ -3527,27 +3766,35 @@
     </row>
     <row r="42" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>2005325450</v>
+        <v>8001244</v>
       </c>
       <c r="B42" s="3">
-        <v>302159005</v>
-      </c>
-      <c r="C42" s="10" t="s">
+        <v>300098723</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="3">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H42" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J42" s="3">
+        <v>3106005200</v>
+      </c>
       <c r="K42" s="3">
         <v>1</v>
       </c>
@@ -3563,15 +3810,21 @@
       <c r="O42" s="3">
         <v>0</v>
       </c>
+      <c r="P42" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R42" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S42" s="3">
         <v>0</v>
       </c>
       <c r="U42" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V42" s="3">
         <f t="shared" si="3"/>
@@ -3580,27 +3833,35 @@
     </row>
     <row r="43" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>2005325450</v>
+        <v>8001244</v>
       </c>
       <c r="B43" s="3">
-        <v>302159005</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>91</v>
+        <v>300098723</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F43" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J43" s="3">
+        <v>3177611859</v>
+      </c>
       <c r="K43" s="3">
         <v>1</v>
       </c>
@@ -3616,15 +3877,21 @@
       <c r="O43" s="3">
         <v>0</v>
       </c>
+      <c r="P43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R43" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S43" s="3">
         <v>0</v>
       </c>
       <c r="U43" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V43" s="3">
         <f t="shared" si="3"/>
@@ -3633,27 +3900,35 @@
     </row>
     <row r="44" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>2005325450</v>
+        <v>8001244</v>
       </c>
       <c r="B44" s="3">
-        <v>302159005</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>92</v>
+        <v>300098723</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H44" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J44" s="3">
+        <v>3048663520</v>
+      </c>
       <c r="K44" s="3">
         <v>1</v>
       </c>
@@ -3669,15 +3944,21 @@
       <c r="O44" s="3">
         <v>0</v>
       </c>
+      <c r="P44" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R44" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S44" s="3">
         <v>0</v>
       </c>
       <c r="U44" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V44" s="3">
         <f t="shared" si="3"/>
@@ -3686,27 +3967,35 @@
     </row>
     <row r="45" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>2005325453</v>
+        <v>100054211</v>
       </c>
       <c r="B45" s="3">
-        <v>302159008</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>93</v>
+        <v>300098722</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="D45" s="3">
         <v>1</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F45" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H45" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J45" s="3">
+        <v>300450233</v>
+      </c>
       <c r="K45" s="3">
         <v>1</v>
       </c>
@@ -3722,15 +4011,21 @@
       <c r="O45" s="3">
         <v>0</v>
       </c>
+      <c r="P45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R45" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S45" s="3">
         <v>0</v>
       </c>
       <c r="U45" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V45" s="3">
         <f t="shared" si="3"/>
@@ -3739,25 +4034,25 @@
     </row>
     <row r="46" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>2005325454</v>
+        <v>1000369852</v>
       </c>
       <c r="B46" s="3">
-        <v>302159009</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>94</v>
+        <v>300098721</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D46" s="3">
         <v>3</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F46" s="3">
         <v>0</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H46" s="3"/>
       <c r="K46" s="3">
@@ -3776,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S46" s="3">
         <v>0</v>
@@ -3792,25 +4087,25 @@
     </row>
     <row r="47" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>2005325455</v>
+        <v>1009658742</v>
       </c>
       <c r="B47" s="3">
-        <v>302159010</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>95</v>
+        <v>300098720</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F47" s="3">
         <v>0</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H47" s="3"/>
       <c r="K47" s="3">
@@ -3829,14 +4124,14 @@
         <v>0</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S47" s="3">
         <v>0</v>
       </c>
       <c r="U47" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V47" s="3">
         <f t="shared" si="3"/>
@@ -3845,25 +4140,25 @@
     </row>
     <row r="48" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>2005325456</v>
+        <v>1000852456</v>
       </c>
       <c r="B48" s="3">
-        <v>302159011</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>96</v>
+        <v>300098719</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F48" s="3">
         <v>0</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H48" s="3"/>
       <c r="K48" s="3">
@@ -3882,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S48" s="3">
         <v>0</v>
@@ -3898,25 +4193,25 @@
     </row>
     <row r="49" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>2005325457</v>
+        <v>1000852456</v>
       </c>
       <c r="B49" s="3">
-        <v>302159012</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>97</v>
+        <v>300098719</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F49" s="3">
         <v>0</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H49" s="3"/>
       <c r="K49" s="3">
@@ -3935,14 +4230,14 @@
         <v>0</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S49" s="3">
         <v>0</v>
       </c>
       <c r="U49" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V49" s="3">
         <f t="shared" si="3"/>
@@ -3951,25 +4246,25 @@
     </row>
     <row r="50" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>2005325458</v>
+        <v>1000852456</v>
       </c>
       <c r="B50" s="3">
-        <v>302159013</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>98</v>
+        <v>300098719</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F50" s="3">
         <v>0</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H50" s="3"/>
       <c r="K50" s="3">
@@ -3988,14 +4283,14 @@
         <v>0</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S50" s="3">
         <v>0</v>
       </c>
       <c r="U50" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V50" s="3">
         <f t="shared" si="3"/>
@@ -4004,27 +4299,26 @@
     </row>
     <row r="51" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>2005325459</v>
+        <v>10005214</v>
       </c>
       <c r="B51" s="3">
-        <v>302159014</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="3">
-        <v>1</v>
+        <v>300098716</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F51" s="3">
         <v>0</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H51" s="3"/>
+        <v>71</v>
+      </c>
       <c r="K51" s="3">
         <v>1</v>
       </c>
@@ -4041,14 +4335,14 @@
         <v>0</v>
       </c>
       <c r="R51" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S51" s="3">
         <v>0</v>
       </c>
       <c r="U51" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V51" s="3">
         <f t="shared" si="3"/>
@@ -4057,27 +4351,35 @@
     </row>
     <row r="52" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>2005325460</v>
+        <v>100096532</v>
       </c>
       <c r="B52" s="3">
-        <v>302159015</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D52" s="3">
-        <v>2</v>
+        <v>300098715</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F52" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H52" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J52" s="3">
+        <v>315952014</v>
+      </c>
       <c r="K52" s="3">
         <v>1</v>
       </c>
@@ -4093,15 +4395,21 @@
       <c r="O52" s="3">
         <v>0</v>
       </c>
+      <c r="P52" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R52" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S52" s="3">
         <v>0</v>
       </c>
       <c r="U52" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V52" s="3">
         <f t="shared" si="3"/>
@@ -4110,27 +4418,35 @@
     </row>
     <row r="53" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>2005325461</v>
+        <v>100082792</v>
       </c>
       <c r="B53" s="3">
-        <v>302159016</v>
+        <v>300098714</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="3">
+        <v>14</v>
+      </c>
+      <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H53" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J53" s="3">
+        <v>315746952</v>
+      </c>
       <c r="K53" s="3">
         <v>1</v>
       </c>
@@ -4146,15 +4462,21 @@
       <c r="O53" s="3">
         <v>0</v>
       </c>
+      <c r="P53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R53" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S53" s="3">
         <v>0</v>
       </c>
       <c r="U53" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V53" s="3">
         <f t="shared" si="3"/>
@@ -4163,25 +4485,34 @@
     </row>
     <row r="54" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>2005325462</v>
+        <v>1000200148</v>
       </c>
       <c r="B54" s="3">
-        <v>302159017</v>
+        <v>300098713</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="3">
+        <v>11</v>
+      </c>
+      <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J54" s="3">
+        <v>300852165</v>
       </c>
       <c r="K54" s="3">
         <v>1</v>
@@ -4198,15 +4529,21 @@
       <c r="O54" s="3">
         <v>0</v>
       </c>
+      <c r="P54" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R54" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S54" s="3">
         <v>0</v>
       </c>
       <c r="U54" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V54" s="3">
         <f t="shared" si="3"/>
@@ -4215,25 +4552,34 @@
     </row>
     <row r="55" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>2005325463</v>
+        <v>50006234</v>
       </c>
       <c r="B55" s="3">
-        <v>302159018</v>
+        <v>300098711</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="3">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="F55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J55" s="3">
+        <v>302654872</v>
       </c>
       <c r="K55" s="3">
         <v>1</v>
@@ -4250,15 +4596,21 @@
       <c r="O55" s="3">
         <v>0</v>
       </c>
+      <c r="P55" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q55" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R55" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S55" s="3">
         <v>0</v>
       </c>
       <c r="U55" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V55" s="3">
         <f t="shared" si="3"/>
@@ -4267,10 +4619,10 @@
     </row>
     <row r="56" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>2005325464</v>
+        <v>50006234</v>
       </c>
       <c r="B56" s="3">
-        <v>302159019</v>
+        <v>300098711</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>11</v>
@@ -4278,14 +4630,23 @@
       <c r="D56">
         <v>1</v>
       </c>
-      <c r="E56" t="s">
-        <v>31</v>
+      <c r="E56" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="F56" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J56" s="3">
+        <v>302654872</v>
       </c>
       <c r="K56" s="3">
         <v>1</v>
@@ -4302,15 +4663,21 @@
       <c r="O56" s="3">
         <v>0</v>
       </c>
+      <c r="P56" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q56" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R56" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S56" s="3">
         <v>0</v>
       </c>
       <c r="U56" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V56" s="3">
         <f t="shared" si="3"/>
@@ -4319,25 +4686,34 @@
     </row>
     <row r="57" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>2005325465</v>
+        <v>50006234</v>
       </c>
       <c r="B57" s="3">
-        <v>302159020</v>
+        <v>300098711</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="D57">
-        <v>3</v>
-      </c>
-      <c r="E57" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="F57" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J57" s="3">
+        <v>302654872</v>
       </c>
       <c r="K57" s="3">
         <v>1</v>
@@ -4354,15 +4730,21 @@
       <c r="O57" s="3">
         <v>0</v>
       </c>
+      <c r="P57" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R57" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S57" s="3">
         <v>0</v>
       </c>
       <c r="U57" s="3">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V57" s="3">
         <f t="shared" si="3"/>
@@ -4371,77 +4753,101 @@
     </row>
     <row r="58" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>2005325466</v>
+        <v>28520012</v>
       </c>
       <c r="B58" s="3">
-        <v>302159021</v>
+        <v>300098709</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F58" s="3">
+        <v>2</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J58" s="3">
+        <v>316803001</v>
+      </c>
+      <c r="K58" s="3">
+        <v>1</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0</v>
+      </c>
+      <c r="M58" s="3">
+        <v>0</v>
+      </c>
+      <c r="N58" s="3">
+        <v>0</v>
+      </c>
+      <c r="O58" s="3">
+        <v>0</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S58" s="3">
+        <v>0</v>
+      </c>
+      <c r="U58" s="3">
+        <f t="shared" ref="U58:U65" si="4">VLOOKUP(E58,T_OPERADORES,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E58" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" s="3">
-        <v>0</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K58" s="3">
-        <v>1</v>
-      </c>
-      <c r="L58" s="3">
-        <v>0</v>
-      </c>
-      <c r="M58" s="3">
-        <v>0</v>
-      </c>
-      <c r="N58" s="3">
-        <v>0</v>
-      </c>
-      <c r="O58" s="3">
-        <v>0</v>
-      </c>
-      <c r="R58" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S58" s="3">
-        <v>0</v>
-      </c>
-      <c r="U58" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
       <c r="V58" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="V58:V65" si="5">VLOOKUP(G58,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>2005325467</v>
+        <v>285213605</v>
       </c>
       <c r="B59" s="3">
-        <v>302159022</v>
+        <v>300098708</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D59">
         <v>2</v>
       </c>
-      <c r="E59" t="s">
-        <v>29</v>
+      <c r="E59" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="F59" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J59" s="3">
+        <v>320464331</v>
       </c>
       <c r="K59" s="3">
         <v>1</v>
@@ -4458,51 +4864,57 @@
       <c r="O59" s="3">
         <v>0</v>
       </c>
+      <c r="P59" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R59" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S59" s="3">
         <v>0</v>
       </c>
       <c r="U59" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="V59" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>2005325468</v>
+        <v>28526490</v>
       </c>
       <c r="B60" s="3">
-        <v>302159023</v>
+        <v>300098707</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F60" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J60" s="3">
-        <v>315952014</v>
+        <v>321932510</v>
       </c>
       <c r="K60" s="3">
         <v>1</v>
@@ -4520,56 +4932,56 @@
         <v>0</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S60" s="3">
         <v>0</v>
       </c>
       <c r="U60" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="V60" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>2005325469</v>
+        <v>28643211</v>
       </c>
       <c r="B61" s="3">
-        <v>302159024</v>
+        <v>300098706</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F61" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J61" s="3">
-        <v>315746952</v>
+        <v>300211548</v>
       </c>
       <c r="K61" s="3">
         <v>1</v>
@@ -4587,56 +4999,56 @@
         <v>0</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R61" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S61" s="3">
         <v>0</v>
       </c>
       <c r="U61" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="V61" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>2005325470</v>
+        <v>279500012</v>
       </c>
       <c r="B62" s="3">
-        <v>302159025</v>
+        <v>300098705</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F62" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>114</v>
+        <v>71</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="J62" s="3">
-        <v>300852165</v>
+        <v>320458695</v>
       </c>
       <c r="K62" s="3">
         <v>1</v>
@@ -4654,56 +5066,56 @@
         <v>0</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q62" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S62" s="3">
         <v>0</v>
       </c>
       <c r="U62" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="V62" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>2005325471</v>
+        <v>246850047</v>
       </c>
       <c r="B63" s="3">
-        <v>302159026</v>
+        <v>300098704</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F63" s="3">
         <v>2</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F63" s="3">
-        <v>1</v>
-      </c>
       <c r="G63" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>115</v>
+        <v>71</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="J63" s="3">
-        <v>302654872</v>
+        <v>3024115687</v>
       </c>
       <c r="K63" s="3">
         <v>1</v>
@@ -4721,56 +5133,56 @@
         <v>0</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S63" s="3">
         <v>0</v>
       </c>
       <c r="U63" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="V63" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <v>2005325471</v>
+        <v>400025652</v>
       </c>
       <c r="B64" s="3">
-        <v>302159026</v>
+        <v>300098703</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F64" s="3">
         <v>2</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>115</v>
+        <v>71</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="J64" s="3">
-        <v>302654872</v>
+        <v>320456322</v>
       </c>
       <c r="K64" s="3">
         <v>1</v>
@@ -4788,56 +5200,56 @@
         <v>0</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S64" s="3">
         <v>0</v>
       </c>
       <c r="U64" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="V64" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>2005325471</v>
+        <v>400025652</v>
       </c>
       <c r="B65" s="3">
-        <v>302159026</v>
+        <v>300098703</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F65" s="3">
         <v>2</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>115</v>
+        <v>71</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="J65" s="3">
-        <v>302654872</v>
+        <v>3115869632</v>
       </c>
       <c r="K65" s="3">
         <v>1</v>
@@ -4855,560 +5267,80 @@
         <v>0</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q65" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S65" s="3">
         <v>0</v>
       </c>
       <c r="U65" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="V65" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3">
-        <v>2005325474</v>
-      </c>
-      <c r="B66" s="3">
-        <v>302159029</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F66" s="3">
-        <v>2</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="J66" s="3">
-        <v>316803001</v>
-      </c>
-      <c r="K66" s="3">
-        <v>1</v>
-      </c>
-      <c r="L66" s="3">
-        <v>0</v>
-      </c>
-      <c r="M66" s="3">
-        <v>0</v>
-      </c>
-      <c r="N66" s="3">
-        <v>0</v>
-      </c>
-      <c r="O66" s="3">
-        <v>0</v>
-      </c>
-      <c r="P66" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R66" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S66" s="3">
-        <v>0</v>
-      </c>
-      <c r="U66" s="3">
-        <f t="shared" ref="U66:U73" si="4">VLOOKUP(E66,T_OPERADORES,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="V66" s="3">
-        <f t="shared" ref="V66:V73" si="5">VLOOKUP(G66,T_TIPO_ENVIO,2,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3">
-        <v>2005325475</v>
-      </c>
-      <c r="B67" s="3">
-        <v>302159030</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F67" s="3">
-        <v>2</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J67" s="3">
-        <v>320464331</v>
-      </c>
-      <c r="K67" s="3">
-        <v>1</v>
-      </c>
-      <c r="L67" s="3">
-        <v>0</v>
-      </c>
-      <c r="M67" s="3">
-        <v>0</v>
-      </c>
-      <c r="N67" s="3">
-        <v>0</v>
-      </c>
-      <c r="O67" s="3">
-        <v>0</v>
-      </c>
-      <c r="P67" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q67" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R67" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S67" s="3">
-        <v>0</v>
-      </c>
-      <c r="U67" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="V67" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3">
-        <v>2005325476</v>
-      </c>
-      <c r="B68" s="3">
-        <v>302159031</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F68" s="3">
-        <v>2</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J68" s="3">
-        <v>321932510</v>
-      </c>
-      <c r="K68" s="3">
-        <v>1</v>
-      </c>
-      <c r="L68" s="3">
-        <v>0</v>
-      </c>
-      <c r="M68" s="3">
-        <v>0</v>
-      </c>
-      <c r="N68" s="3">
-        <v>0</v>
-      </c>
-      <c r="O68" s="3">
-        <v>0</v>
-      </c>
-      <c r="P68" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q68" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R68" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S68" s="3">
-        <v>0</v>
-      </c>
-      <c r="U68" s="3">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="V68" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3">
-        <v>2005325477</v>
-      </c>
-      <c r="B69" s="3">
-        <v>302159032</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F69" s="3">
-        <v>2</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J69" s="3">
-        <v>300211548</v>
-      </c>
-      <c r="K69" s="3">
-        <v>1</v>
-      </c>
-      <c r="L69" s="3">
-        <v>0</v>
-      </c>
-      <c r="M69" s="3">
-        <v>0</v>
-      </c>
-      <c r="N69" s="3">
-        <v>0</v>
-      </c>
-      <c r="O69" s="3">
-        <v>0</v>
-      </c>
-      <c r="P69" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q69" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R69" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S69" s="3">
-        <v>0</v>
-      </c>
-      <c r="U69" s="3">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="V69" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3">
-        <v>2005325478</v>
-      </c>
-      <c r="B70" s="3">
-        <v>302159033</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
-        <v>29</v>
-      </c>
-      <c r="F70" s="3">
-        <v>0</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H70" s="3"/>
-      <c r="K70" s="3">
-        <v>1</v>
-      </c>
-      <c r="L70" s="3">
-        <v>0</v>
-      </c>
-      <c r="M70" s="3">
-        <v>0</v>
-      </c>
-      <c r="N70" s="3">
-        <v>0</v>
-      </c>
-      <c r="O70" s="3">
-        <v>0</v>
-      </c>
-      <c r="R70" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S70" s="3">
-        <v>0</v>
-      </c>
-      <c r="U70" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V70" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3">
-        <v>2005325479</v>
-      </c>
-      <c r="B71" s="3">
-        <v>302159034</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>29</v>
-      </c>
-      <c r="F71" s="3">
-        <v>0</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K71" s="3">
-        <v>1</v>
-      </c>
-      <c r="L71" s="3">
-        <v>0</v>
-      </c>
-      <c r="M71" s="3">
-        <v>0</v>
-      </c>
-      <c r="N71" s="3">
-        <v>0</v>
-      </c>
-      <c r="O71" s="3">
-        <v>0</v>
-      </c>
-      <c r="R71" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S71" s="3">
-        <v>0</v>
-      </c>
-      <c r="U71" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V71" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3">
-        <v>2005325480</v>
-      </c>
-      <c r="B72" s="3">
-        <v>302159035</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D72">
-        <v>2</v>
-      </c>
-      <c r="E72" t="s">
-        <v>29</v>
-      </c>
-      <c r="F72" s="3">
-        <v>0</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K72" s="3">
-        <v>1</v>
-      </c>
-      <c r="L72" s="3">
-        <v>0</v>
-      </c>
-      <c r="M72" s="3">
-        <v>0</v>
-      </c>
-      <c r="N72" s="3">
-        <v>0</v>
-      </c>
-      <c r="O72" s="3">
-        <v>0</v>
-      </c>
-      <c r="R72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S72" s="3">
-        <v>0</v>
-      </c>
-      <c r="U72" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V72" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3">
-        <v>2005325480</v>
-      </c>
-      <c r="B73" s="3">
-        <v>302159035</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73" t="s">
-        <v>29</v>
-      </c>
-      <c r="F73" s="3">
-        <v>0</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K73" s="3">
-        <v>1</v>
-      </c>
-      <c r="L73" s="3">
-        <v>0</v>
-      </c>
-      <c r="M73" s="3">
-        <v>0</v>
-      </c>
-      <c r="N73" s="3">
-        <v>0</v>
-      </c>
-      <c r="O73" s="3">
-        <v>0</v>
-      </c>
-      <c r="R73" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S73" s="3">
-        <v>0</v>
-      </c>
-      <c r="U73" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V73" s="3">
+      <c r="V65" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="17" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C38">
-    <cfRule type="duplicateValues" dxfId="16" priority="19"/>
+  <conditionalFormatting sqref="C2:C37">
+    <cfRule type="duplicateValues" dxfId="32" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="duplicateValues" dxfId="31" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C55">
-    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="duplicateValues" dxfId="30" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C61">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="duplicateValues" dxfId="29" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="duplicateValues" dxfId="28" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C61">
+    <cfRule type="duplicateValues" dxfId="27" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C61">
+    <cfRule type="duplicateValues" dxfId="26" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65:C69">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  <conditionalFormatting sqref="C56 C1:C37 C62 C66:C1048576 C51:C54">
+    <cfRule type="duplicateValues" dxfId="22" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65:C69">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="C66:C1048576 C1:C37 C51:C63">
+    <cfRule type="duplicateValues" dxfId="21" priority="33"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="C64:C65">
+    <cfRule type="duplicateValues" dxfId="20" priority="37"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="C51:C53">
+    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="B2:B65">
+    <cfRule type="duplicateValues" dxfId="18" priority="42"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B73">
-    <cfRule type="duplicateValues" dxfId="3" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C38 C64 C70 C74:C1048576 C53:C62">
-    <cfRule type="duplicateValues" dxfId="2" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C38 C74:C1048576 C53:C71">
-    <cfRule type="duplicateValues" dxfId="1" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C72:C73">
-    <cfRule type="duplicateValues" dxfId="0" priority="36"/>
+  <conditionalFormatting sqref="C2:C65">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5431,24 +5363,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="D1" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="13"/>
+      <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -5456,13 +5388,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -5470,7 +5402,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -5478,7 +5410,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -5486,7 +5418,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -5494,7 +5426,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>

</xml_diff>

<commit_message>
correccion de errores menores
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
+++ b/Files/Temp_alist_adm/900987412_3/900987412_3_1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\LOGI\Carga Masiva\Masivo Inventario Alistamiento\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -15,7 +20,7 @@
     <definedName name="T_OPERADORES">Hoja2!$A$1:$B$8</definedName>
     <definedName name="T_TIPO_ENVIO">Hoja2!$D$1:$E$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -26,7 +31,7 @@
     <author>Andres</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -42,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1">
+    <comment ref="K1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1">
+    <comment ref="P1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1">
+    <comment ref="Q1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +420,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -964,7 +969,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -999,7 +1004,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1212,7 +1217,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>